<commit_message>
DOcumentação -Atualização na Análise de Valor agregado
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Cost Performance Index</t>
+  </si>
+  <si>
+    <t>Sprint planejado</t>
   </si>
 </sst>
 </file>
@@ -278,8 +281,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -329,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -352,6 +355,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -364,62 +378,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <condense val="0"/>
@@ -513,21 +498,21 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.5</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122.5</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
@@ -675,32 +660,32 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80197888"/>
-        <c:axId val="80203776"/>
+        <c:axId val="73067520"/>
+        <c:axId val="73077504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80197888"/>
+        <c:axId val="73067520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80203776"/>
+        <c:crossAx val="73077504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80203776"/>
+        <c:axId val="73077504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80197888"/>
+        <c:crossAx val="73067520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -713,7 +698,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1039,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1052,9 +1037,10 @@
     <col min="3" max="3" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
     <col min="5" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1082,8 +1068,11 @@
       <c r="I1" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1116,8 +1105,11 @@
         <f t="shared" ref="I2" si="1">H2</f>
         <v>S</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1150,8 +1142,11 @@
         <f t="shared" ref="I3:I63" si="6">H3</f>
         <v>S</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1184,8 +1179,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1218,8 +1216,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1251,8 +1252,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1285,8 +1289,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1317,8 +1324,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1349,8 +1359,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1383,8 +1396,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1416,8 +1432,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1449,8 +1468,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1482,8 +1504,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1515,8 +1540,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1548,8 +1576,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1581,8 +1612,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -1613,8 +1647,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1647,8 +1684,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1680,8 +1720,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1713,8 +1756,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1746,8 +1792,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1780,8 +1829,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1813,8 +1865,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1846,8 +1901,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1879,8 +1937,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1912,8 +1973,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1945,8 +2009,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1978,8 +2045,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2011,8 +2081,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2044,8 +2117,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2077,8 +2153,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2110,8 +2189,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2143,8 +2225,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2176,8 +2261,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2209,8 +2297,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2242,8 +2333,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2275,8 +2369,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2308,8 +2405,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2341,8 +2441,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2373,8 +2476,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2406,8 +2512,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2439,8 +2548,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2471,8 +2583,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2503,8 +2618,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2536,8 +2654,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2569,8 +2690,11 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -2601,8 +2725,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -2635,8 +2762,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="4" t="s">
         <v>49</v>
       </c>
@@ -2666,8 +2796,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="4" t="s">
         <v>50</v>
       </c>
@@ -2697,8 +2830,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="4" t="s">
         <v>51</v>
       </c>
@@ -2728,8 +2864,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
         <v>52</v>
       </c>
@@ -2759,8 +2898,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
         <v>53</v>
       </c>
@@ -2790,8 +2932,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
         <v>54</v>
       </c>
@@ -2821,8 +2966,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
@@ -2852,8 +3000,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
@@ -2883,8 +3034,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
@@ -2914,8 +3068,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -2945,8 +3102,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
         <v>59</v>
       </c>
@@ -2976,8 +3136,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
         <v>60</v>
       </c>
@@ -3009,8 +3172,11 @@
       <c r="I60" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -3040,8 +3206,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
@@ -3073,8 +3242,11 @@
       <c r="I62" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -3105,8 +3277,11 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="10" t="s">
         <v>66</v>
       </c>
@@ -3121,6 +3296,24 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="4"/>
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3">
+        <v>2</v>
+      </c>
+      <c r="F65" s="3">
+        <v>3</v>
+      </c>
+      <c r="G65" s="3">
+        <v>4</v>
+      </c>
+      <c r="H65" s="3">
+        <v>5</v>
+      </c>
+      <c r="I65" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="4"/>
@@ -3152,27 +3345,27 @@
         <v>76</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:G67" si="7">E67-$I$67/6</f>
-        <v>24.5</v>
+        <f>SUMIF($J$2:$J$63,"&lt;="&amp;D65,$C$2:$C$63)</f>
+        <v>13.5</v>
       </c>
       <c r="E67">
-        <f t="shared" si="7"/>
-        <v>49</v>
+        <f t="shared" ref="E67:I67" si="7">SUMIF($J$2:$J$63,"&lt;="&amp;E65,$C$2:$C$63)</f>
+        <v>36.5</v>
       </c>
       <c r="F67">
         <f t="shared" si="7"/>
-        <v>73.5</v>
+        <v>52.5</v>
       </c>
       <c r="G67">
         <f t="shared" si="7"/>
-        <v>98</v>
+        <v>64.5</v>
       </c>
       <c r="H67">
-        <f>I67-$I$67/6</f>
-        <v>122.5</v>
-      </c>
-      <c r="I67" s="11">
-        <f>C64</f>
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="7"/>
         <v>147</v>
       </c>
     </row>
@@ -3250,28 +3443,28 @@
       <c r="C70" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="14">
+      <c r="D70" s="11">
         <f>D68/D67</f>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="E70" s="14">
-        <f t="shared" ref="E70:I70" si="10">E68/E67</f>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F70" s="14">
-        <f t="shared" si="10"/>
-        <v>0.48299319727891155</v>
-      </c>
-      <c r="G70" s="14">
-        <f t="shared" si="10"/>
-        <v>0.45408163265306123</v>
-      </c>
-      <c r="H70" s="14">
-        <f t="shared" si="10"/>
-        <v>0.58775510204081638</v>
-      </c>
-      <c r="I70" s="14">
-        <f t="shared" si="10"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E70" s="11">
+        <f>E68/E67</f>
+        <v>0.57534246575342463</v>
+      </c>
+      <c r="F70" s="11">
+        <f>F68/F67</f>
+        <v>0.67619047619047623</v>
+      </c>
+      <c r="G70" s="11">
+        <f>G68/G67</f>
+        <v>0.68992248062015504</v>
+      </c>
+      <c r="H70" s="11">
+        <f>H68/H67</f>
+        <v>0.75</v>
+      </c>
+      <c r="I70" s="11">
+        <f>I68/I67</f>
         <v>0.51020408163265307</v>
       </c>
     </row>
@@ -3283,28 +3476,28 @@
       <c r="C71" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="14">
+      <c r="D71" s="11">
         <f>D68/D69</f>
         <v>0.95454545454545459</v>
       </c>
-      <c r="E71" s="14">
-        <f t="shared" ref="E71:I71" si="11">E68/E69</f>
+      <c r="E71" s="11">
+        <f t="shared" ref="E71:I71" si="10">E68/E69</f>
         <v>0.875</v>
       </c>
-      <c r="F71" s="14">
-        <f t="shared" si="11"/>
+      <c r="F71" s="11">
+        <f t="shared" si="10"/>
         <v>0.86585365853658536</v>
       </c>
-      <c r="G71" s="14">
-        <f t="shared" si="11"/>
+      <c r="G71" s="11">
+        <f t="shared" si="10"/>
         <v>0.80909090909090908</v>
       </c>
-      <c r="H71" s="14">
-        <f t="shared" si="11"/>
+      <c r="H71" s="11">
+        <f t="shared" si="10"/>
         <v>0.81355932203389836</v>
       </c>
-      <c r="I71" s="14">
-        <f t="shared" si="11"/>
+      <c r="I71" s="11">
+        <f t="shared" si="10"/>
         <v>0.81081081081081086</v>
       </c>
     </row>
@@ -3317,13 +3510,13 @@
     <mergeCell ref="A71:B71"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:I63">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Alteração em documentação e tela objetivo -Mudança no label de objetivo -Alteração na analise de valor agregado e burndown
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visagio\git\BatalhaDoPassinho\Documentação\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="10455" windowHeight="4620"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -160,9 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mostrar objetivos: </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t xml:space="preserve">dar opção de jogar com a IA: </t>
@@ -279,12 +281,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,13 +395,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,17 +438,37 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -518,6 +540,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -581,11 +604,12 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -653,39 +677,57 @@
                   <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.5</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="73067520"/>
-        <c:axId val="73077504"/>
+        <c:smooth val="0"/>
+        <c:axId val="114781584"/>
+        <c:axId val="114782144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73067520"/>
+        <c:axId val="114781584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73077504"/>
+        <c:crossAx val="114782144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73077504"/>
+        <c:axId val="114782144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73067520"/>
+        <c:crossAx val="114781584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -693,8 +735,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -782,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -814,9 +859,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -848,6 +894,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1023,14 +1070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:J15"/>
+    <sheetView tabSelected="1" topLeftCell="C64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="9"/>
@@ -1040,7 +1087,7 @@
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,28 +1098,28 @@
         <v>45</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="J1" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1083,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:H2" si="0">D2</f>
@@ -1109,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E63" si="2">D3</f>
@@ -1146,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1157,7 +1204,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="2"/>
@@ -1183,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1241,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
@@ -1220,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1231,14 +1278,14 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="4"/>
@@ -1256,7 +1303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="2"/>
@@ -1293,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1349,7 @@
         <v>2.5</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="2"/>
@@ -1328,7 +1375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1384,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="2"/>
@@ -1363,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1374,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="2"/>
@@ -1400,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1411,10 +1458,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="3"/>
@@ -1436,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1447,10 +1494,10 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="3"/>
@@ -1472,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1483,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="3"/>
@@ -1508,7 +1555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1519,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="3"/>
@@ -1544,9 +1591,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
@@ -1555,10 +1602,10 @@
         <v>2.5</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
@@ -1580,9 +1627,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7">
         <v>1.5</v>
@@ -1591,7 +1638,7 @@
         <v>2.5</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="2"/>
@@ -1606,7 +1653,7 @@
         <v>N</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="6"/>
@@ -1616,16 +1663,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7">
         <v>2.5</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="2"/>
@@ -1651,7 +1698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1662,7 +1709,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="2"/>
@@ -1688,7 +1735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1699,14 +1746,14 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="4"/>
@@ -1724,7 +1771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1735,14 +1782,14 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="4"/>
@@ -1760,7 +1807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1771,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="2"/>
@@ -1782,7 +1829,7 @@
         <v>N</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="5"/>
@@ -1796,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1807,7 +1854,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="2"/>
@@ -1833,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1844,7 +1891,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="2"/>
@@ -1859,7 +1906,7 @@
         <v>N</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="6"/>
@@ -1869,7 +1916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1927,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="2"/>
@@ -1891,7 +1938,7 @@
         <v>N</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="5"/>
@@ -1905,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1916,14 +1963,14 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="4"/>
@@ -1941,7 +1988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1952,14 +1999,14 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="4"/>
@@ -1977,7 +2024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1988,14 +2035,14 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="4"/>
@@ -2013,7 +2060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2024,10 +2071,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="3"/>
@@ -2049,7 +2096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2060,14 +2107,14 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="4"/>
@@ -2085,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2096,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="2"/>
@@ -2111,7 +2158,7 @@
         <v>N</v>
       </c>
       <c r="H30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="6"/>
@@ -2121,7 +2168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2132,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="2"/>
@@ -2147,7 +2194,7 @@
         <v>N</v>
       </c>
       <c r="H31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="6"/>
@@ -2157,7 +2204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2168,7 +2215,7 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="2"/>
@@ -2183,7 +2230,7 @@
         <v>N</v>
       </c>
       <c r="H32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="6"/>
@@ -2193,7 +2240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2204,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="2"/>
@@ -2219,7 +2266,7 @@
         <v>N</v>
       </c>
       <c r="H33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="6"/>
@@ -2229,7 +2276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2240,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="2"/>
@@ -2255,7 +2302,7 @@
         <v>N</v>
       </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="6"/>
@@ -2265,7 +2312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2276,7 +2323,7 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="2"/>
@@ -2291,7 +2338,7 @@
         <v>N</v>
       </c>
       <c r="H35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="6"/>
@@ -2301,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2312,14 +2359,14 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="4"/>
@@ -2337,7 +2384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2348,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="2"/>
@@ -2359,7 +2406,7 @@
         <v>N</v>
       </c>
       <c r="G37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="5"/>
@@ -2373,7 +2420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2384,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="2"/>
@@ -2395,7 +2442,7 @@
         <v>N</v>
       </c>
       <c r="G38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="5"/>
@@ -2409,7 +2456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2420,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="2"/>
@@ -2431,7 +2478,7 @@
         <v>N</v>
       </c>
       <c r="G39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="5"/>
@@ -2445,7 +2492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2456,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="2"/>
@@ -2467,10 +2514,10 @@
         <v>N</v>
       </c>
       <c r="G40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="6"/>
@@ -2480,7 +2527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2491,7 +2538,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="2"/>
@@ -2506,7 +2553,7 @@
         <v>N</v>
       </c>
       <c r="H41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="6"/>
@@ -2516,7 +2563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2527,14 +2574,14 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="4"/>
@@ -2552,7 +2599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2561,7 +2608,7 @@
         <v>5.5</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="2"/>
@@ -2587,7 +2634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2596,7 +2643,7 @@
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="2"/>
@@ -2622,7 +2669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2633,14 +2680,14 @@
         <v>0.5</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
       </c>
       <c r="F45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="4"/>
@@ -2658,7 +2705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2669,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="2"/>
@@ -2684,7 +2731,7 @@
         <v>N</v>
       </c>
       <c r="H46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="6"/>
@@ -2694,7 +2741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -2703,7 +2750,7 @@
         <v>4.5</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="2"/>
@@ -2729,18 +2776,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>48</v>
+      <c r="B48" s="8">
+        <v>0.5</v>
       </c>
       <c r="C48" s="7">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="2"/>
@@ -2758,23 +2805,22 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I48" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I48" t="s">
+        <v>73</v>
       </c>
       <c r="J48">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="9">
         <v>2.5</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="2"/>
@@ -2800,15 +2846,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" s="9">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="2"/>
@@ -2834,15 +2880,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" s="9">
         <v>3.5</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="2"/>
@@ -2868,15 +2914,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="9">
         <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="2"/>
@@ -2902,15 +2948,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" s="9">
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="2"/>
@@ -2936,15 +2982,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="9">
         <v>3.5</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="2"/>
@@ -2970,15 +3016,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" s="9">
         <v>3.5</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="2"/>
@@ -3004,15 +3050,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="9">
         <v>3.5</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="2"/>
@@ -3038,15 +3084,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" s="9">
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="2"/>
@@ -3072,15 +3118,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C58" s="9">
         <v>2.5</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="2"/>
@@ -3106,15 +3152,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" s="9">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="2"/>
@@ -3140,9 +3186,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="9">
         <v>3</v>
@@ -3151,7 +3197,7 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="2"/>
@@ -3170,21 +3216,21 @@
         <v>N</v>
       </c>
       <c r="I60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J60">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" s="9">
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="2"/>
@@ -3210,9 +3256,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="9">
         <v>1</v>
@@ -3221,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="2"/>
@@ -3240,13 +3286,13 @@
         <v>N</v>
       </c>
       <c r="I62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J62">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -3255,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="2"/>
@@ -3281,20 +3327,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" s="9">
         <f>SUM(B2:B63)</f>
-        <v>92.5</v>
+        <v>93</v>
       </c>
       <c r="C64" s="9">
         <f>SUM(C2:C63)</f>
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="D65" s="3">
         <v>1</v>
@@ -3315,34 +3361,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="D66" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="F66" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="G66" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="H66" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="I66" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I66" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="12" t="s">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="D67">
         <f>SUMIF($J$2:$J$63,"&lt;="&amp;D65,$C$2:$C$63)</f>
@@ -3369,13 +3415,13 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="12" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="D68" s="3">
         <f>SUMIF(D2:D63,"=S",$C$2:$C$63)</f>
@@ -3399,16 +3445,16 @@
       </c>
       <c r="I68" s="3">
         <f t="shared" si="8"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="13"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" s="14"/>
       <c r="C69" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D69" s="3">
         <f>SUMIF(D2:D63,"=S",$B$2:$B$63)</f>
@@ -3432,73 +3478,73 @@
       </c>
       <c r="I69" s="3">
         <f t="shared" si="9"/>
-        <v>92.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="11">
+        <f t="shared" ref="D70:I70" si="10">D68/D67</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E70" s="11">
+        <f t="shared" si="10"/>
+        <v>0.57534246575342463</v>
+      </c>
+      <c r="F70" s="11">
+        <f t="shared" si="10"/>
+        <v>0.67619047619047623</v>
+      </c>
+      <c r="G70" s="11">
+        <f t="shared" si="10"/>
+        <v>0.68992248062015504</v>
+      </c>
+      <c r="H70" s="11">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="I70" s="11">
+        <f t="shared" si="10"/>
+        <v>0.52380952380952384</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="11">
-        <f>D68/D67</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="E70" s="11">
-        <f>E68/E67</f>
-        <v>0.57534246575342463</v>
-      </c>
-      <c r="F70" s="11">
-        <f>F68/F67</f>
-        <v>0.67619047619047623</v>
-      </c>
-      <c r="G70" s="11">
-        <f>G68/G67</f>
-        <v>0.68992248062015504</v>
-      </c>
-      <c r="H70" s="11">
-        <f>H68/H67</f>
-        <v>0.75</v>
-      </c>
-      <c r="I70" s="11">
-        <f>I68/I67</f>
-        <v>0.51020408163265307</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" s="13"/>
-      <c r="C71" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="D71" s="11">
         <f>D68/D69</f>
         <v>0.95454545454545459</v>
       </c>
       <c r="E71" s="11">
-        <f t="shared" ref="E71:I71" si="10">E68/E69</f>
+        <f t="shared" ref="E71:I71" si="11">E68/E69</f>
         <v>0.875</v>
       </c>
       <c r="F71" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.86585365853658536</v>
       </c>
       <c r="G71" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.80909090909090908</v>
       </c>
       <c r="H71" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.81355932203389836</v>
       </c>
       <c r="I71" s="11">
-        <f t="shared" si="10"/>
-        <v>0.81081081081081086</v>
+        <f t="shared" si="11"/>
+        <v>0.82795698924731187</v>
       </c>
     </row>
   </sheetData>
@@ -3527,24 +3573,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Organização de pacotes + javadoc + Documentação -Organização dos pacotes da IA -JavaDoc nos métodos e classes do pacote IA -Atualização do burndown e valor agregado
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -13,15 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="85">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -604,7 +602,7 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>77</c:v>
+                  <c:v>93.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,7 +675,7 @@
                   <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,11 +692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114781584"/>
-        <c:axId val="114782144"/>
+        <c:axId val="125260000"/>
+        <c:axId val="125260560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114781584"/>
+        <c:axId val="125260000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114782144"/>
+        <c:crossAx val="125260560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -717,7 +715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114782144"/>
+        <c:axId val="125260560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,7 +725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114781584"/>
+        <c:crossAx val="125260000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1073,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,7 +2601,9 @@
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="7"/>
+      <c r="B43" s="7">
+        <v>8</v>
+      </c>
       <c r="C43" s="7">
         <v>5.5</v>
       </c>
@@ -2626,9 +2626,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I43" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I43" t="s">
+        <v>73</v>
       </c>
       <c r="J43">
         <v>5</v>
@@ -2638,7 +2637,9 @@
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="7"/>
+      <c r="B44" s="7">
+        <v>4</v>
+      </c>
       <c r="C44" s="7">
         <v>4</v>
       </c>
@@ -2661,9 +2662,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I44" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I44" t="s">
+        <v>73</v>
       </c>
       <c r="J44">
         <v>6</v>
@@ -2745,7 +2745,9 @@
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="7">
+        <v>3.5</v>
+      </c>
       <c r="C47" s="7">
         <v>4.5</v>
       </c>
@@ -2768,9 +2770,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I47" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I47" t="s">
+        <v>73</v>
       </c>
       <c r="J47">
         <v>5</v>
@@ -2816,6 +2817,9 @@
       <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B49" s="9">
+        <v>0.5</v>
+      </c>
       <c r="C49" s="9">
         <v>2.5</v>
       </c>
@@ -2838,9 +2842,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I49" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I49" t="s">
+        <v>73</v>
       </c>
       <c r="J49">
         <v>6</v>
@@ -3333,7 +3336,7 @@
       </c>
       <c r="B64" s="9">
         <f>SUM(B2:B63)</f>
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C64" s="9">
         <f>SUM(C2:C63)</f>
@@ -3445,7 +3448,7 @@
       </c>
       <c r="I68" s="3">
         <f t="shared" si="8"/>
-        <v>77</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3478,7 +3481,7 @@
       </c>
       <c r="I69" s="3">
         <f t="shared" si="9"/>
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3511,7 +3514,7 @@
       </c>
       <c r="I70" s="11">
         <f t="shared" si="10"/>
-        <v>0.52380952380952384</v>
+        <v>0.63605442176870752</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,7 +3547,7 @@
       </c>
       <c r="I71" s="11">
         <f t="shared" si="11"/>
-        <v>0.82795698924731187</v>
+        <v>0.85779816513761464</v>
       </c>
     </row>
   </sheetData>
@@ -3570,28 +3573,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Documentação -Atualização do BurnDown e Valor Agregado
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -602,7 +602,7 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93.5</c:v>
+                  <c:v>99.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,7 +675,7 @@
                   <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,11 +692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="125260000"/>
-        <c:axId val="125260560"/>
+        <c:axId val="126443936"/>
+        <c:axId val="126444496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125260000"/>
+        <c:axId val="126443936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125260560"/>
+        <c:crossAx val="126444496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -715,7 +715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125260560"/>
+        <c:axId val="126444496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125260000"/>
+        <c:crossAx val="126443936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,6 +3057,9 @@
       <c r="A56" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="B56" s="9">
+        <v>5</v>
+      </c>
       <c r="C56" s="9">
         <v>3.5</v>
       </c>
@@ -3079,9 +3082,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I56" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I56" t="s">
+        <v>73</v>
       </c>
       <c r="J56">
         <v>6</v>
@@ -3125,6 +3127,9 @@
       <c r="A58" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
       <c r="C58" s="9">
         <v>2.5</v>
       </c>
@@ -3147,9 +3152,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I58" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I58" t="s">
+        <v>73</v>
       </c>
       <c r="J58">
         <v>6</v>
@@ -3336,7 +3340,7 @@
       </c>
       <c r="B64" s="9">
         <f>SUM(B2:B63)</f>
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C64" s="9">
         <f>SUM(C2:C63)</f>
@@ -3448,7 +3452,7 @@
       </c>
       <c r="I68" s="3">
         <f t="shared" si="8"/>
-        <v>93.5</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3481,7 +3485,7 @@
       </c>
       <c r="I69" s="3">
         <f t="shared" si="9"/>
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3514,7 +3518,7 @@
       </c>
       <c r="I70" s="11">
         <f t="shared" si="10"/>
-        <v>0.63605442176870752</v>
+        <v>0.6768707482993197</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3547,7 +3551,7 @@
       </c>
       <c r="I71" s="11">
         <f t="shared" si="11"/>
-        <v>0.85779816513761464</v>
+        <v>0.86521739130434783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementação do HighLight nos botões e documentação
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="85">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -602,7 +602,7 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.5</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,7 +675,7 @@
                   <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>115</c:v>
+                  <c:v>119.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,11 +692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126443936"/>
-        <c:axId val="126444496"/>
+        <c:axId val="116481824"/>
+        <c:axId val="116482384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126443936"/>
+        <c:axId val="116481824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126444496"/>
+        <c:crossAx val="116482384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -715,7 +715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126444496"/>
+        <c:axId val="116482384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126443936"/>
+        <c:crossAx val="116481824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3023,6 +3023,9 @@
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B55" s="9">
+        <v>0.5</v>
+      </c>
       <c r="C55" s="9">
         <v>3.5</v>
       </c>
@@ -3045,9 +3048,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I55" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I55" t="s">
+        <v>73</v>
       </c>
       <c r="J55">
         <v>6</v>
@@ -3163,6 +3165,9 @@
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B59" s="9">
+        <v>2</v>
+      </c>
       <c r="C59" s="9">
         <v>3</v>
       </c>
@@ -3185,9 +3190,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I59" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I59" t="s">
+        <v>73</v>
       </c>
       <c r="J59">
         <v>6</v>
@@ -3233,6 +3237,9 @@
       <c r="A61" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B61" s="9">
+        <v>2</v>
+      </c>
       <c r="C61" s="9">
         <v>3</v>
       </c>
@@ -3255,9 +3262,8 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I61" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
+      <c r="I61" t="s">
+        <v>73</v>
       </c>
       <c r="J61">
         <v>6</v>
@@ -3340,7 +3346,7 @@
       </c>
       <c r="B64" s="9">
         <f>SUM(B2:B63)</f>
-        <v>115</v>
+        <v>119.5</v>
       </c>
       <c r="C64" s="9">
         <f>SUM(C2:C63)</f>
@@ -3452,7 +3458,7 @@
       </c>
       <c r="I68" s="3">
         <f t="shared" si="8"/>
-        <v>99.5</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3485,7 +3491,7 @@
       </c>
       <c r="I69" s="3">
         <f t="shared" si="9"/>
-        <v>115</v>
+        <v>119.5</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3518,7 +3524,7 @@
       </c>
       <c r="I70" s="11">
         <f t="shared" si="10"/>
-        <v>0.6768707482993197</v>
+        <v>0.74149659863945583</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3551,7 +3557,7 @@
       </c>
       <c r="I71" s="11">
         <f t="shared" si="11"/>
-        <v>0.86521739130434783</v>
+        <v>0.91213389121338917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentação -Atualização do BurnDown e Valor Agregado -Apresentação 3º seminario
</commit_message>
<xml_diff>
--- a/Documentação/Análise de Valor Agregado.xlsx
+++ b/Documentação/Análise de Valor Agregado.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visagio\git\BatalhaDoPassinho\Documentação\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="10455" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="91">
   <si>
     <t>Nome da tarefa</t>
   </si>
@@ -274,17 +269,35 @@
   </si>
   <si>
     <t>Sprint planejado</t>
+  </si>
+  <si>
+    <t>Sprint 7</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Tarefas de Refatoração e acompanhamento</t>
+  </si>
+  <si>
+    <t>Reuniões</t>
+  </si>
+  <si>
+    <t>Casos de Teste</t>
+  </si>
+  <si>
+    <t>Testes Unitários</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,7 +417,152 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -449,30 +607,18 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$67</c:f>
+              <c:f>Plan1!$C$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -487,9 +633,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$D$66:$I$66</c:f>
+              <c:f>Plan1!$D$70:$J$70</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -507,16 +653,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$67:$I$67</c:f>
+              <c:f>Plan1!$D$71:$J$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>13.5</c:v>
                 </c:pt>
@@ -534,18 +683,20 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$68</c:f>
+              <c:f>Plan1!$C$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -556,9 +707,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$D$66:$I$66</c:f>
+              <c:f>Plan1!$D$70:$J$70</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -576,16 +727,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$68:$I$68</c:f>
+              <c:f>Plan1!$D$72:$J$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10.5</c:v>
                 </c:pt>
@@ -602,19 +756,21 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109</c:v>
+                  <c:v>121.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$69</c:f>
+              <c:f>Plan1!$C$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -629,9 +785,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$D$66:$I$66</c:f>
+              <c:f>Plan1!$D$70:$J$70</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -649,16 +805,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Sprint 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sprint 7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$69:$I$69</c:f>
+              <c:f>Plan1!$D$73:$J$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -675,57 +834,44 @@
                   <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>119.5</c:v>
+                  <c:v>138.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="116481824"/>
-        <c:axId val="116482384"/>
+        <c:axId val="45171072"/>
+        <c:axId val="45172608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116481824"/>
+        <c:axId val="45171072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116482384"/>
+        <c:crossAx val="45172608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116482384"/>
+        <c:axId val="45172608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116481824"/>
+        <c:crossAx val="45171072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -733,15 +879,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -752,15 +896,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3160059</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
+      <xdr:colOff>2442021</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>112921</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>347383</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -825,7 +969,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -857,10 +1001,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -892,7 +1035,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1068,24 +1210,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="9"/>
     <col min="3" max="3" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
     <col min="5" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1113,11 +1256,14 @@
       <c r="I1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1150,11 +1296,15 @@
         <f t="shared" ref="I2" si="1">H2</f>
         <v>S</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="str">
+        <f>I2</f>
+        <v>S</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1184,14 +1334,18 @@
         <v>S</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I63" si="6">H3</f>
-        <v>S</v>
-      </c>
-      <c r="J3">
+        <f t="shared" ref="I3:I57" si="6">H3</f>
+        <v>S</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J62" si="7">I3</f>
+        <v>S</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1224,11 +1378,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1261,11 +1419,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1297,11 +1459,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1334,15 +1500,21 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
       <c r="C8" s="7">
         <v>2.5</v>
       </c>
@@ -1369,15 +1541,20 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
       <c r="C9" s="7">
         <v>3</v>
       </c>
@@ -1404,11 +1581,14 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1441,11 +1621,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1477,11 +1661,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1513,11 +1701,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1549,11 +1741,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1585,11 +1781,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J14">
+      <c r="J14" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -1621,11 +1821,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J15">
+      <c r="J15" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1657,15 +1861,21 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J16">
+      <c r="J16" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7">
+        <v>2</v>
+      </c>
       <c r="C17" s="7">
         <v>2.5</v>
       </c>
@@ -1692,11 +1902,14 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J17">
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1729,11 +1942,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J18">
+      <c r="J18" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1765,11 +1982,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J19">
+      <c r="J19" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1801,11 +2022,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J20">
+      <c r="J20" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1837,11 +2062,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J21">
+      <c r="J21" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1874,11 +2103,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J22">
+      <c r="J22" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1910,11 +2143,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J23">
+      <c r="J23" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1946,11 +2183,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J24">
+      <c r="J24" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1982,11 +2223,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J25">
+      <c r="J25" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2018,11 +2263,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J26">
+      <c r="J26" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2054,11 +2303,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J27">
+      <c r="J27" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2090,11 +2343,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J28">
+      <c r="J28" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2126,11 +2383,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J29">
+      <c r="J29" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2162,11 +2423,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J30">
+      <c r="J30" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2198,11 +2463,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J31">
+      <c r="J31" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2234,11 +2503,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J32">
+      <c r="J32" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2270,11 +2543,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J33">
+      <c r="J33" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2306,11 +2583,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J34">
+      <c r="J34" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -2342,11 +2623,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J35">
+      <c r="J35" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K35">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2378,11 +2663,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J36">
+      <c r="J36" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2414,11 +2703,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J37">
+      <c r="J37" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2450,11 +2743,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J38">
+      <c r="J38" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2486,11 +2783,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J39">
+      <c r="J39" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2521,11 +2822,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J40">
+      <c r="J40" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2557,11 +2862,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J41">
+      <c r="J41" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K41">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2593,11 +2902,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J42">
+      <c r="J42" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2629,11 +2942,15 @@
       <c r="I43" t="s">
         <v>73</v>
       </c>
-      <c r="J43">
+      <c r="J43" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K43">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2665,11 +2982,15 @@
       <c r="I44" t="s">
         <v>73</v>
       </c>
-      <c r="J44">
+      <c r="J44" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K44">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2701,11 +3022,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J45">
+      <c r="J45" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2737,11 +3062,15 @@
         <f t="shared" si="6"/>
         <v>S</v>
       </c>
-      <c r="J46">
+      <c r="J46" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -2773,11 +3102,15 @@
       <c r="I47" t="s">
         <v>73</v>
       </c>
-      <c r="J47">
+      <c r="J47" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K47">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -2809,11 +3142,15 @@
       <c r="I48" t="s">
         <v>73</v>
       </c>
-      <c r="J48">
+      <c r="J48" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K48">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" s="4" t="s">
         <v>48</v>
       </c>
@@ -2845,14 +3182,21 @@
       <c r="I49" t="s">
         <v>73</v>
       </c>
-      <c r="J49">
+      <c r="J49" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K49">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="B50" s="9">
+        <v>6</v>
+      </c>
       <c r="C50" s="9">
         <v>5</v>
       </c>
@@ -2879,14 +3223,20 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J50">
+      <c r="J50" t="s">
+        <v>73</v>
+      </c>
+      <c r="K50">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B51" s="9">
+        <v>5</v>
+      </c>
       <c r="C51" s="9">
         <v>3.5</v>
       </c>
@@ -2909,18 +3259,24 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I51" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J51">
+      <c r="I51" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K51">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="B52" s="9">
+        <v>5</v>
+      </c>
       <c r="C52" s="9">
         <v>6</v>
       </c>
@@ -2943,18 +3299,23 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I52" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J52">
+      <c r="I52" t="s">
+        <v>72</v>
+      </c>
+      <c r="J52" t="s">
+        <v>86</v>
+      </c>
+      <c r="K52">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
       <c r="C53" s="9">
         <v>6</v>
       </c>
@@ -2977,18 +3338,24 @@
         <f t="shared" si="5"/>
         <v>N</v>
       </c>
-      <c r="I53" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J53">
+      <c r="I53" t="s">
+        <v>73</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="B54" s="9">
+        <v>8</v>
+      </c>
       <c r="C54" s="9">
         <v>3.5</v>
       </c>
@@ -3015,11 +3382,14 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J54">
+      <c r="J54" t="s">
+        <v>73</v>
+      </c>
+      <c r="K54">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -3051,11 +3421,15 @@
       <c r="I55" t="s">
         <v>73</v>
       </c>
-      <c r="J55">
+      <c r="J55" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K55">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56" s="4" t="s">
         <v>55</v>
       </c>
@@ -3087,14 +3461,21 @@
       <c r="I56" t="s">
         <v>73</v>
       </c>
-      <c r="J56">
+      <c r="J56" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K56">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="B57" s="9">
+        <v>2</v>
+      </c>
       <c r="C57" s="9">
         <v>3</v>
       </c>
@@ -3121,11 +3502,14 @@
         <f t="shared" si="6"/>
         <v>N</v>
       </c>
-      <c r="J57">
+      <c r="J57" t="s">
+        <v>73</v>
+      </c>
+      <c r="K57">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58" s="4" t="s">
         <v>57</v>
       </c>
@@ -3157,11 +3541,15 @@
       <c r="I58" t="s">
         <v>73</v>
       </c>
-      <c r="J58">
+      <c r="J58" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K58">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -3193,11 +3581,15 @@
       <c r="I59" t="s">
         <v>73</v>
       </c>
-      <c r="J59">
+      <c r="J59" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K59">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="A60" s="4" t="s">
         <v>59</v>
       </c>
@@ -3229,11 +3621,15 @@
       <c r="I60" t="s">
         <v>73</v>
       </c>
-      <c r="J60">
+      <c r="J60" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K60">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="A61" s="4" t="s">
         <v>60</v>
       </c>
@@ -3265,11 +3661,15 @@
       <c r="I61" t="s">
         <v>73</v>
       </c>
-      <c r="J61">
+      <c r="J61" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K61">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
@@ -3301,15 +3701,21 @@
       <c r="I62" t="s">
         <v>73</v>
       </c>
-      <c r="J62">
+      <c r="J62" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="K62">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="7"/>
+      <c r="B63" s="7">
+        <v>0.5</v>
+      </c>
       <c r="C63" s="7">
         <v>3</v>
       </c>
@@ -3317,265 +3723,462 @@
         <v>72</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="2"/>
+        <f>D63</f>
         <v>N</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="3"/>
+        <f>E63</f>
         <v>N</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="4"/>
+        <f>F63</f>
         <v>N</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="5"/>
-        <v>N</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="6"/>
-        <v>N</v>
-      </c>
-      <c r="J63">
+        <f>G63</f>
+        <v>N</v>
+      </c>
+      <c r="I63" t="s">
+        <v>73</v>
+      </c>
+      <c r="J63" t="str">
+        <f>I63</f>
+        <v>S</v>
+      </c>
+      <c r="K63">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+    <row r="64" spans="1:11">
+      <c r="A64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="7">
+        <v>3</v>
+      </c>
+      <c r="C64" s="7">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>72</v>
+      </c>
+      <c r="E64" t="str">
+        <f>D64</f>
+        <v>N</v>
+      </c>
+      <c r="F64" t="str">
+        <f>E64</f>
+        <v>N</v>
+      </c>
+      <c r="G64" t="str">
+        <f>F64</f>
+        <v>N</v>
+      </c>
+      <c r="H64" t="str">
+        <f>G64</f>
+        <v>N</v>
+      </c>
+      <c r="I64" t="s">
+        <v>72</v>
+      </c>
+      <c r="J64" t="s">
+        <v>73</v>
+      </c>
+      <c r="K64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" s="7">
+        <v>3</v>
+      </c>
+      <c r="C65" s="7">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65" t="str">
+        <f>D65</f>
+        <v>N</v>
+      </c>
+      <c r="F65" t="str">
+        <f>E65</f>
+        <v>N</v>
+      </c>
+      <c r="G65" t="str">
+        <f>F65</f>
+        <v>N</v>
+      </c>
+      <c r="H65" t="str">
+        <f>G65</f>
+        <v>N</v>
+      </c>
+      <c r="I65" t="s">
+        <v>72</v>
+      </c>
+      <c r="J65" t="s">
+        <v>73</v>
+      </c>
+      <c r="K65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>72</v>
+      </c>
+      <c r="E66" t="str">
+        <f>D66</f>
+        <v>N</v>
+      </c>
+      <c r="F66" t="str">
+        <f>E66</f>
+        <v>N</v>
+      </c>
+      <c r="G66" t="str">
+        <f>F66</f>
+        <v>N</v>
+      </c>
+      <c r="H66" t="str">
+        <f>G66</f>
+        <v>N</v>
+      </c>
+      <c r="I66" t="s">
+        <v>73</v>
+      </c>
+      <c r="J66" t="str">
+        <f>I66</f>
+        <v>S</v>
+      </c>
+      <c r="K66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="7">
+        <v>20</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>72</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67" si="8">D67</f>
+        <v>N</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" ref="F67" si="9">E67</f>
+        <v>N</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67" si="10">F67</f>
+        <v>N</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" ref="H67" si="11">G67</f>
+        <v>N</v>
+      </c>
+      <c r="I67" t="s">
+        <v>72</v>
+      </c>
+      <c r="J67" t="s">
+        <v>73</v>
+      </c>
+      <c r="K67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="9">
-        <f>SUM(B2:B63)</f>
-        <v>119.5</v>
-      </c>
-      <c r="C64" s="9">
-        <f>SUM(C2:C63)</f>
+      <c r="B68" s="9">
+        <f>SUM(B2:B67)</f>
+        <v>193.5</v>
+      </c>
+      <c r="C68" s="9">
+        <f>SUM(C2:C67)</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="4"/>
+      <c r="D69" s="3">
+        <v>1</v>
+      </c>
+      <c r="E69" s="3">
+        <v>2</v>
+      </c>
+      <c r="F69" s="3">
+        <v>3</v>
+      </c>
+      <c r="G69" s="3">
+        <v>4</v>
+      </c>
+      <c r="H69" s="3">
+        <v>5</v>
+      </c>
+      <c r="I69" s="3">
+        <v>6</v>
+      </c>
+      <c r="J69" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="4"/>
+      <c r="D70" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D71">
+        <f>SUMIF($K$2:$K$67,"&lt;="&amp;D69,$C$2:$C$67)</f>
+        <v>13.5</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ref="E71:I71" si="12">SUMIF($K$2:$K$67,"&lt;="&amp;E69,$C$2:$C$67)</f>
+        <v>36.5</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="12"/>
+        <v>52.5</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="12"/>
+        <v>64.5</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="12"/>
+        <v>96</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="12"/>
         <v>147</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="D65" s="3">
+      <c r="J71">
+        <f>SUMIF($K$2:$K$67,"&lt;="&amp;J69,$C$2:$C$67)</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D72" s="3">
+        <f>SUMIF(D2:D67,"=S",$C$2:$C$67)</f>
+        <v>10.5</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" ref="E72:J72" si="13">SUMIF(E2:E67,"=S",$C$2:$C$67)</f>
+        <v>21</v>
+      </c>
+      <c r="F72" s="3">
+        <f t="shared" si="13"/>
+        <v>35.5</v>
+      </c>
+      <c r="G72" s="3">
+        <f t="shared" si="13"/>
+        <v>44.5</v>
+      </c>
+      <c r="H72" s="3">
+        <f t="shared" si="13"/>
+        <v>72</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="13"/>
+        <v>121.5</v>
+      </c>
+      <c r="J72" s="3">
+        <f t="shared" si="13"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="C73" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="3">
+        <f>SUMIF(D2:D67,"=S",$B$2:$B$67)</f>
+        <v>11</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" ref="E73:J73" si="14">SUMIF(E2:E67,"=S",$B$2:$B$67)</f>
+        <v>24</v>
+      </c>
+      <c r="F73" s="3">
+        <f t="shared" si="14"/>
+        <v>41</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" si="14"/>
+        <v>55</v>
+      </c>
+      <c r="H73" s="3">
+        <f t="shared" si="14"/>
+        <v>88.5</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="14"/>
+        <v>138.5</v>
+      </c>
+      <c r="J73" s="3">
+        <f t="shared" si="14"/>
+        <v>193.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="11">
+        <f t="shared" ref="D74:I74" si="15">D72/D71</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E74" s="11">
+        <f t="shared" si="15"/>
+        <v>0.57534246575342463</v>
+      </c>
+      <c r="F74" s="11">
+        <f t="shared" si="15"/>
+        <v>0.67619047619047623</v>
+      </c>
+      <c r="G74" s="11">
+        <f t="shared" si="15"/>
+        <v>0.68992248062015504</v>
+      </c>
+      <c r="H74" s="11">
+        <f t="shared" si="15"/>
+        <v>0.75</v>
+      </c>
+      <c r="I74" s="11">
+        <f t="shared" si="15"/>
+        <v>0.82653061224489799</v>
+      </c>
+      <c r="J74" s="11">
+        <f t="shared" ref="J74" si="16">J72/J71</f>
         <v>1</v>
       </c>
-      <c r="E65" s="3">
-        <v>2</v>
-      </c>
-      <c r="F65" s="3">
-        <v>3</v>
-      </c>
-      <c r="G65" s="3">
-        <v>4</v>
-      </c>
-      <c r="H65" s="3">
-        <v>5</v>
-      </c>
-      <c r="I65" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="D66" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H66" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I66" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D67">
-        <f>SUMIF($J$2:$J$63,"&lt;="&amp;D65,$C$2:$C$63)</f>
-        <v>13.5</v>
-      </c>
-      <c r="E67">
-        <f t="shared" ref="E67:I67" si="7">SUMIF($J$2:$J$63,"&lt;="&amp;E65,$C$2:$C$63)</f>
-        <v>36.5</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="7"/>
-        <v>52.5</v>
-      </c>
-      <c r="G67">
-        <f t="shared" si="7"/>
-        <v>64.5</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="7"/>
-        <v>96</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="7"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" s="13"/>
-      <c r="C68" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="3">
-        <f>SUMIF(D2:D63,"=S",$C$2:$C$63)</f>
-        <v>10.5</v>
-      </c>
-      <c r="E68" s="3">
-        <f t="shared" ref="E68:I68" si="8">SUMIF(E2:E63,"=S",$C$2:$C$63)</f>
-        <v>21</v>
-      </c>
-      <c r="F68" s="3">
-        <f t="shared" si="8"/>
-        <v>35.5</v>
-      </c>
-      <c r="G68" s="3">
-        <f t="shared" si="8"/>
-        <v>44.5</v>
-      </c>
-      <c r="H68" s="3">
-        <f t="shared" si="8"/>
-        <v>72</v>
-      </c>
-      <c r="I68" s="3">
-        <f t="shared" si="8"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B69" s="14"/>
-      <c r="C69" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D69" s="3">
-        <f>SUMIF(D2:D63,"=S",$B$2:$B$63)</f>
-        <v>11</v>
-      </c>
-      <c r="E69" s="3">
-        <f t="shared" ref="E69:I69" si="9">SUMIF(E2:E63,"=S",$B$2:$B$63)</f>
-        <v>24</v>
-      </c>
-      <c r="F69" s="3">
-        <f t="shared" si="9"/>
-        <v>41</v>
-      </c>
-      <c r="G69" s="3">
-        <f t="shared" si="9"/>
-        <v>55</v>
-      </c>
-      <c r="H69" s="3">
-        <f t="shared" si="9"/>
-        <v>88.5</v>
-      </c>
-      <c r="I69" s="3">
-        <f t="shared" si="9"/>
-        <v>119.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="14"/>
-      <c r="C70" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D70" s="11">
-        <f t="shared" ref="D70:I70" si="10">D68/D67</f>
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="E70" s="11">
-        <f t="shared" si="10"/>
-        <v>0.57534246575342463</v>
-      </c>
-      <c r="F70" s="11">
-        <f t="shared" si="10"/>
-        <v>0.67619047619047623</v>
-      </c>
-      <c r="G70" s="11">
-        <f t="shared" si="10"/>
-        <v>0.68992248062015504</v>
-      </c>
-      <c r="H70" s="11">
-        <f t="shared" si="10"/>
-        <v>0.75</v>
-      </c>
-      <c r="I70" s="11">
-        <f t="shared" si="10"/>
-        <v>0.74149659863945583</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="14"/>
-      <c r="C71" s="9" t="s">
+      <c r="B75" s="14"/>
+      <c r="C75" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D71" s="11">
-        <f>D68/D69</f>
+      <c r="D75" s="11">
+        <f>D72/D73</f>
         <v>0.95454545454545459</v>
       </c>
-      <c r="E71" s="11">
-        <f t="shared" ref="E71:I71" si="11">E68/E69</f>
+      <c r="E75" s="11">
+        <f t="shared" ref="E75:I75" si="17">E72/E73</f>
         <v>0.875</v>
       </c>
-      <c r="F71" s="11">
-        <f t="shared" si="11"/>
+      <c r="F75" s="11">
+        <f t="shared" si="17"/>
         <v>0.86585365853658536</v>
       </c>
-      <c r="G71" s="11">
-        <f t="shared" si="11"/>
+      <c r="G75" s="11">
+        <f t="shared" si="17"/>
         <v>0.80909090909090908</v>
       </c>
-      <c r="H71" s="11">
-        <f t="shared" si="11"/>
+      <c r="H75" s="11">
+        <f t="shared" si="17"/>
         <v>0.81355932203389836</v>
       </c>
-      <c r="I71" s="11">
-        <f t="shared" si="11"/>
-        <v>0.91213389121338917</v>
+      <c r="I75" s="11">
+        <f t="shared" si="17"/>
+        <v>0.87725631768953072</v>
+      </c>
+      <c r="J75" s="11">
+        <f t="shared" ref="J75" si="18">J72/J73</f>
+        <v>0.78552971576227393</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
     <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2:I63">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="D2:J62 D64:J67">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="S">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="S">
       <formula>NOT(ISERROR(SEARCH("S",D2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:J63">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="S">
+      <formula>NOT(ISERROR(SEARCH("S",D63)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>